<commit_message>
updated ir_data to fix range error. updated markdown file added a shiny app
</commit_message>
<xml_diff>
--- a/ir_data.xlsx
+++ b/ir_data.xlsx
@@ -432,7 +432,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -458,7 +460,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -528,7 +530,7 @@
         <v>1</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -797,7 +799,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -831,16 +835,15 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
-        <f ca="1" xml:space="preserve"> RANDBETWEEN(100, 999)</f>
-        <v>999</v>
+        <v>627</v>
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -854,16 +857,15 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
-        <f t="shared" ref="A3:A20" ca="1" si="0" xml:space="preserve"> RANDBETWEEN(100, 999)</f>
-        <v>352</v>
+        <v>460</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:C20" ca="1" si="1">RANDBETWEEN(0,100)</f>
-        <v>5</v>
+        <f t="shared" ref="B3:C20" ca="1" si="0">RANDBETWEEN(0,100)</f>
+        <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -877,16 +879,15 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
-        <f t="shared" ca="1" si="0"/>
-        <v>970</v>
+        <v>278</v>
       </c>
       <c r="B4">
-        <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
       </c>
       <c r="C4">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -900,16 +901,15 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
-        <f t="shared" ca="1" si="0"/>
-        <v>143</v>
+        <v>218</v>
       </c>
       <c r="B5">
-        <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
       </c>
       <c r="C5">
-        <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -923,16 +923,15 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
-        <f t="shared" ca="1" si="0"/>
-        <v>828</v>
+        <v>639</v>
       </c>
       <c r="B6">
-        <f t="shared" ca="1" si="1"/>
-        <v>92</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43</v>
       </c>
       <c r="C6">
-        <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -946,16 +945,15 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
-        <f t="shared" ca="1" si="0"/>
-        <v>738</v>
+        <v>962</v>
       </c>
       <c r="B7">
-        <f t="shared" ca="1" si="1"/>
-        <v>63</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
       </c>
       <c r="C7">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -969,16 +967,15 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
-        <f t="shared" ca="1" si="0"/>
-        <v>732</v>
+        <v>836</v>
       </c>
       <c r="B8">
-        <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>60</v>
       </c>
       <c r="C8">
-        <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -992,16 +989,15 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
-        <f t="shared" ca="1" si="0"/>
-        <v>633</v>
+        <v>382</v>
       </c>
       <c r="B9">
-        <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
       </c>
       <c r="C9">
-        <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -1015,15 +1011,14 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
-        <f t="shared" ca="1" si="0"/>
-        <v>827</v>
+        <v>187</v>
       </c>
       <c r="B10">
-        <f t="shared" ca="1" si="1"/>
-        <v>46</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
       </c>
       <c r="C10">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>97</v>
       </c>
       <c r="D10" t="s">
@@ -1038,16 +1033,15 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
-        <f t="shared" ca="1" si="0"/>
-        <v>354</v>
+        <v>170</v>
       </c>
       <c r="B11">
-        <f t="shared" ca="1" si="1"/>
-        <v>57</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>97</v>
       </c>
       <c r="C11">
-        <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -1061,16 +1055,15 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
-        <f t="shared" ca="1" si="0"/>
-        <v>809</v>
+        <v>238</v>
       </c>
       <c r="B12">
-        <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>49</v>
       </c>
       <c r="C12">
-        <f t="shared" ca="1" si="1"/>
-        <v>63</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
@@ -1084,16 +1077,15 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
-        <f t="shared" ca="1" si="0"/>
-        <v>465</v>
+        <v>976</v>
       </c>
       <c r="B13">
-        <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
       </c>
       <c r="C13">
-        <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -1107,16 +1099,15 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
-        <f t="shared" ca="1" si="0"/>
-        <v>692</v>
+        <v>959</v>
       </c>
       <c r="B14">
-        <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
       </c>
       <c r="C14">
-        <f t="shared" ca="1" si="1"/>
-        <v>91</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -1130,16 +1121,15 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
-        <f t="shared" ca="1" si="0"/>
-        <v>788</v>
+        <v>497</v>
       </c>
       <c r="B15">
-        <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
       </c>
       <c r="C15">
-        <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
@@ -1153,16 +1143,15 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
-        <f t="shared" ca="1" si="0"/>
-        <v>178</v>
+        <v>840</v>
       </c>
       <c r="B16">
-        <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>36</v>
       </c>
       <c r="C16">
-        <f t="shared" ca="1" si="1"/>
-        <v>94</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
@@ -1176,16 +1165,15 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
-        <f t="shared" ca="1" si="0"/>
-        <v>862</v>
+        <v>596</v>
       </c>
       <c r="B17">
-        <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>49</v>
       </c>
       <c r="C17">
-        <f t="shared" ca="1" si="1"/>
-        <v>41</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -1199,16 +1187,15 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
-        <f t="shared" ca="1" si="0"/>
-        <v>437</v>
+        <v>212</v>
       </c>
       <c r="B18">
-        <f t="shared" ca="1" si="1"/>
-        <v>96</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
       </c>
       <c r="C18">
-        <f t="shared" ca="1" si="1"/>
-        <v>97</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
@@ -1222,16 +1209,15 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
-        <f t="shared" ca="1" si="0"/>
-        <v>141</v>
+        <v>611</v>
       </c>
       <c r="B19">
-        <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>52</v>
       </c>
       <c r="C19">
-        <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
@@ -1245,16 +1231,15 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
-        <f t="shared" ca="1" si="0"/>
-        <v>631</v>
+        <v>864</v>
       </c>
       <c r="B20">
-        <f t="shared" ca="1" si="1"/>
-        <v>95</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
       </c>
       <c r="C20">
-        <f t="shared" ca="1" si="1"/>
-        <v>41</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>96</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>

</xml_diff>